<commit_message>
task completely runs successfully
</commit_message>
<xml_diff>
--- a/task/src/main/java/resources/ObjectRepository.xlsx
+++ b/task/src/main/java/resources/ObjectRepository.xlsx
@@ -70,9 +70,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>dropdownLanguage</t>
-  </si>
-  <si>
     <t>english option</t>
   </si>
   <si>
@@ -82,10 +79,13 @@
     <t>Sign Up</t>
   </si>
   <si>
-    <t>Xpath</t>
-  </si>
-  <si>
     <t>//button[text()=' Sign Up']</t>
+  </si>
+  <si>
+    <t>dropdownLangauge</t>
+  </si>
+  <si>
+    <t>xpath</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,29 +542,29 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>